<commit_message>
uploading more files for test
</commit_message>
<xml_diff>
--- a/Sample/Connector_with_Googledrive.xlsx
+++ b/Sample/Connector_with_Googledrive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumi.okubo-shuman\AppData\Local\Programs\Git\Memsource_Connector_Test_001\Sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0BC4D5-0B97-481A-959E-5D9D5F3D5617}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2533FEBB-6B44-4F6C-85A1-A6E0291F7B3A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="3810" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="690" windowWidth="15660" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UPDATED" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="180">
   <si>
     <t>Path</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Inizia</t>
   </si>
   <si>
-    <t>スタート</t>
-  </si>
-  <si>
     <t>시작</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>Accedi</t>
   </si>
   <si>
-    <t>ログイン</t>
-  </si>
-  <si>
     <t>로그인</t>
   </si>
   <si>
@@ -208,9 +202,6 @@
   </si>
   <si>
     <t>Da capo</t>
-  </si>
-  <si>
-    <t>リセット</t>
   </si>
   <si>
     <t>재설정</t>
@@ -967,8 +958,8 @@
   </sheetPr>
   <dimension ref="A1:ZZ30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3794,26 +3785,24 @@
       <c r="H4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="17"/>
+      <c r="J4" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="K4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="L4" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="M4" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="N4" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="O4" s="21" t="s">
         <v>41</v>
-      </c>
-      <c r="O4" s="21" t="s">
-        <v>42</v>
       </c>
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
@@ -4508,46 +4497,44 @@
         <v>29</v>
       </c>
       <c r="B5" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="D5" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="G5" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="H5" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="I5" s="17"/>
+      <c r="J5" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="K5" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="L5" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="M5" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="N5" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="O5" s="21" t="s">
         <v>53</v>
-      </c>
-      <c r="N5" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="O5" s="21" t="s">
-        <v>55</v>
       </c>
       <c r="P5" s="13"/>
       <c r="Q5" s="13"/>
@@ -5242,46 +5229,44 @@
         <v>29</v>
       </c>
       <c r="B6" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="F6" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="17" t="s">
+      <c r="G6" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="H6" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="I6" s="17"/>
+      <c r="J6" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="K6" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="L6" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="M6" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="N6" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="O6" s="21" t="s">
         <v>65</v>
-      </c>
-      <c r="M6" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="N6" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="O6" s="21" t="s">
-        <v>68</v>
       </c>
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
@@ -5973,49 +5958,49 @@
     </row>
     <row r="7" spans="1:702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="F7" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="G7" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="17" t="s">
+      <c r="H7" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="I7" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="J7" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="K7" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="L7" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="M7" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="N7" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="O7" s="21" t="s">
         <v>79</v>
-      </c>
-      <c r="M7" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="N7" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="O7" s="21" t="s">
-        <v>82</v>
       </c>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
@@ -6707,49 +6692,49 @@
     </row>
     <row r="8" spans="1:702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B8" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="G8" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="17" t="s">
+      <c r="H8" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="I8" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="J8" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="K8" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="L8" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="M8" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="N8" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="O8" s="21" t="s">
         <v>92</v>
-      </c>
-      <c r="M8" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="N8" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="O8" s="21" t="s">
-        <v>95</v>
       </c>
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
@@ -7441,49 +7426,49 @@
     </row>
     <row r="9" spans="1:702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B9" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="G9" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" s="17" t="s">
+      <c r="H9" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="I9" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="J9" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="K9" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="L9" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="M9" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="N9" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="L9" s="17" t="s">
+      <c r="O9" s="21" t="s">
         <v>105</v>
-      </c>
-      <c r="M9" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="N9" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="O9" s="21" t="s">
-        <v>108</v>
       </c>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
@@ -8175,49 +8160,49 @@
     </row>
     <row r="10" spans="1:702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B10" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="I10" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="F10" s="17" t="s">
+      <c r="J10" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="H10" s="17" t="s">
+      <c r="K10" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="L10" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="J10" s="18" t="s">
+      <c r="M10" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="17" t="s">
+      <c r="N10" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="17" t="s">
+      <c r="O10" s="21" t="s">
         <v>116</v>
-      </c>
-      <c r="M10" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="N10" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="O10" s="21" t="s">
-        <v>119</v>
       </c>
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
@@ -8909,49 +8894,49 @@
     </row>
     <row r="11" spans="1:702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="G11" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="I11" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="J11" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="F11" s="17" t="s">
+      <c r="K11" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="G11" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="I11" s="17" t="s">
+      <c r="L11" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="J11" s="18" t="s">
+      <c r="M11" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="N11" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="O11" s="21" t="s">
         <v>126</v>
-      </c>
-      <c r="L11" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="M11" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="N11" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="O11" s="21" t="s">
-        <v>129</v>
       </c>
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
@@ -9643,49 +9628,49 @@
     </row>
     <row r="12" spans="1:702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B12" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="F12" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="G12" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="D12" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="E12" s="17" t="s">
+      <c r="H12" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="I12" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="J12" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="K12" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="L12" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="M12" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="N12" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="O12" s="21" t="s">
         <v>138</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="M12" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="N12" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="O12" s="21" t="s">
-        <v>141</v>
       </c>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
@@ -10377,49 +10362,49 @@
     </row>
     <row r="13" spans="1:702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="F13" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="G13" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="E13" s="17" t="s">
+      <c r="H13" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="I13" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="J13" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="K13" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="L13" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="J13" s="18" t="s">
+      <c r="M13" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="K13" s="17" t="s">
+      <c r="N13" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="L13" s="17" t="s">
+      <c r="O13" s="21" t="s">
         <v>152</v>
-      </c>
-      <c r="M13" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="N13" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="O13" s="21" t="s">
-        <v>155</v>
       </c>
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
@@ -11111,49 +11096,49 @@
     </row>
     <row r="14" spans="1:702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F14" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="C14" s="17" t="s">
+      <c r="G14" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="D14" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="E14" s="17" t="s">
+      <c r="H14" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="I14" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="J14" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="K14" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="L14" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="M14" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="K14" s="17" t="s">
+      <c r="N14" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="L14" s="17" t="s">
+      <c r="O14" s="21" t="s">
         <v>165</v>
-      </c>
-      <c r="M14" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="N14" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="O14" s="21" t="s">
-        <v>168</v>
       </c>
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
@@ -23121,8 +23106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D98CA0E6-FF0C-43BD-B52E-23AE718D1D47}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.7109375" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23133,62 +23118,62 @@
         <v>2</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B2" s="27"/>
       <c r="C2" s="27" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>176</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>177</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>

</xml_diff>